<commit_message>
Added SQL to csv lineage
</commit_message>
<xml_diff>
--- a/Lineage-Files/SQL_LINEAGE.xlsx
+++ b/Lineage-Files/SQL_LINEAGE.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mountanalytics-my.sharepoint.com/personal/jurriaan_groot_mountanalytics_nl/Documents/Bureaublad/NN/Lineage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MátéKaiser\Github\Lineage_trackers\sql-code-parser\Lineage-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="8_{71890AA2-167D-4428-A68F-3AA2E1F87338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E25508B3-F472-43C2-ADF3-68C992B08B6B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D1A073-ADDB-4520-86DF-265A3E6C2A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="855" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2E6AC758-1CC8-4CE1-825F-5AF038431A36}"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2E6AC758-1CC8-4CE1-825F-5AF038431A36}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad4" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3073" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="378">
   <si>
     <t>ROW_ID</t>
   </si>
@@ -1267,7 +1267,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5624,10 +5624,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3FDA18-BDC6-43FB-89D1-25C6B7F2C85D}">
-  <dimension ref="A1:Q270"/>
+  <dimension ref="A1:Q272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A242" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L272" sqref="L272"/>
+    <sheetView tabSelected="1" topLeftCell="A240" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C267" sqref="C267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -20019,6 +20019,94 @@
         <v>345</v>
       </c>
     </row>
+    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A271" s="2">
+        <v>265</v>
+      </c>
+      <c r="B271" s="2">
+        <f>VLOOKUP(SQL_LINEAGE!F271,SQL_LINEAGE_LABELS!$C$1:$D$999,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F271" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G271" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H271" s="2">
+        <f>VLOOKUP(SQL_LINEAGE!L271,SQL_LINEAGE_LABELS!$C$1:$D$999,2,FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="I271" s="2" t="str">
+        <f t="shared" ref="I271:I272" si="15">L271&amp;"@"&amp;M271</f>
+        <v>EmployeeTerritories_Extract.csv@EmployeeID</v>
+      </c>
+      <c r="J271" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="K271" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="L271" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M271" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A272" s="2">
+        <v>266</v>
+      </c>
+      <c r="B272" s="2">
+        <f>VLOOKUP(SQL_LINEAGE!F272,SQL_LINEAGE_LABELS!$C$1:$D$999,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F272" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G272" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H272" s="2">
+        <f>VLOOKUP(SQL_LINEAGE!L272,SQL_LINEAGE_LABELS!$C$1:$D$999,2,FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="I272" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>EmployeeTerritories_Extract.csv@TerritoryID</v>
+      </c>
+      <c r="J272" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="K272" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="L272" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="M272" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20733,6 +20821,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="46be734d-eb4c-4292-a77e-674ed2ee61f1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009BA60A36B45C17479D03F2FE44859793" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8e4c09f5ccef915c6d224c6c7d646e5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="46be734d-eb4c-4292-a77e-674ed2ee61f1" xmlns:ns4="dcd5c2ca-01f0-4956-a351-2c69587d1cb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2125427a8745b353dc952473de6032c2" ns3:_="" ns4:_="">
     <xsd:import namespace="46be734d-eb4c-4292-a77e-674ed2ee61f1"/>
@@ -20965,24 +21070,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD9A43C0-19CE-4F8E-8785-8744C71D4B93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="46be734d-eb4c-4292-a77e-674ed2ee61f1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dcd5c2ca-01f0-4956-a351-2c69587d1cb0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="46be734d-eb4c-4292-a77e-674ed2ee61f1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5542AFC4-889F-4E0B-9549-938C043F49F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C0049A-33DD-469B-851A-2CCD037E2B05}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20999,29 +21112,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5542AFC4-889F-4E0B-9549-938C043F49F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD9A43C0-19CE-4F8E-8785-8744C71D4B93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="46be734d-eb4c-4292-a77e-674ed2ee61f1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dcd5c2ca-01f0-4956-a351-2c69587d1cb0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update SQL lineage table
</commit_message>
<xml_diff>
--- a/Lineage-Files/SQL_LINEAGE.xlsx
+++ b/Lineage-Files/SQL_LINEAGE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ErwinSiegers\Documents\GitHub\sql-code-parser\Lineage-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ErwinSiegers\Documents\Clients\NN\sankey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF5B239-B748-4CDB-8164-471483D7A72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAF44F9-A0DC-43AF-BFA1-F3449A6B99F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{2E6AC758-1CC8-4CE1-825F-5AF038431A36}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId6"/>
+    <pivotCache cacheId="7" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8573" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8585" uniqueCount="254">
   <si>
     <t>ROW_ID</t>
   </si>
@@ -4743,7 +4743,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E1391EEC-76B0-4454-BF1C-444529905F5F}" name="Draaitabel1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E1391EEC-76B0-4454-BF1C-444529905F5F}" name="Draaitabel1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -5312,8 +5312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3FDA18-BDC6-43FB-89D1-25C6B7F2C85D}">
   <dimension ref="A1:S859"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G436" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N446" sqref="N446"/>
+    <sheetView tabSelected="1" topLeftCell="A813" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B859" sqref="B859"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.8" x14ac:dyDescent="0.25"/>
@@ -50808,9 +50808,9 @@
       <c r="G835" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="H835" s="8" t="e">
+      <c r="H835" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J835,SQL_LINEAGE!L835),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>328</v>
       </c>
       <c r="I835" s="8" t="str">
         <f t="shared" si="34"/>
@@ -50868,9 +50868,9 @@
       <c r="G836" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="H836" s="2" t="e">
+      <c r="H836" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J836,SQL_LINEAGE!L836),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>328</v>
       </c>
       <c r="I836" s="2" t="str">
         <f t="shared" si="34"/>
@@ -50925,9 +50925,9 @@
       <c r="G837" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="H837" s="2" t="e">
+      <c r="H837" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J837,SQL_LINEAGE!L837),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>328</v>
       </c>
       <c r="I837" s="2" t="str">
         <f t="shared" si="34"/>
@@ -50982,9 +50982,9 @@
       <c r="G838" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="H838" s="2" t="e">
+      <c r="H838" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J838,SQL_LINEAGE!L838),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>328</v>
       </c>
       <c r="I838" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51039,9 +51039,9 @@
       <c r="G839" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H839" s="2" t="e">
+      <c r="H839" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J839,SQL_LINEAGE!L839),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>329</v>
       </c>
       <c r="I839" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51094,8 +51094,9 @@
       <c r="G840" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="H840" s="13" t="e">
-        <v>#N/A</v>
+      <c r="H840" s="2">
+        <f>VLOOKUP(_xlfn.CONCAT(J840,SQL_LINEAGE!L840),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
+        <v>329</v>
       </c>
       <c r="I840" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51150,9 +51151,9 @@
       <c r="G841" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="H841" s="2" t="e">
+      <c r="H841" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J841,SQL_LINEAGE!L841),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>329</v>
       </c>
       <c r="I841" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51207,9 +51208,9 @@
       <c r="G842" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="H842" s="2" t="e">
+      <c r="H842" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J842,SQL_LINEAGE!L842),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>329</v>
       </c>
       <c r="I842" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51264,9 +51265,9 @@
       <c r="G843" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H843" s="2" t="e">
+      <c r="H843" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J843,SQL_LINEAGE!L843),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>329</v>
       </c>
       <c r="I843" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51321,9 +51322,9 @@
       <c r="G844" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H844" s="2" t="e">
+      <c r="H844" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J844,SQL_LINEAGE!L844),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>329</v>
       </c>
       <c r="I844" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51378,9 +51379,9 @@
       <c r="G845" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="H845" s="2" t="e">
+      <c r="H845" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J845,SQL_LINEAGE!L845),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>329</v>
       </c>
       <c r="I845" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51435,9 +51436,9 @@
       <c r="G846" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H846" s="2" t="e">
+      <c r="H846" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J846,SQL_LINEAGE!L846),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>329</v>
       </c>
       <c r="I846" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51492,9 +51493,9 @@
       <c r="G847" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H847" s="2" t="e">
+      <c r="H847" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J847,SQL_LINEAGE!L847),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>330</v>
       </c>
       <c r="I847" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51547,9 +51548,9 @@
       <c r="G848" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H848" s="2" t="e">
+      <c r="H848" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J848,SQL_LINEAGE!L848),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>330</v>
       </c>
       <c r="I848" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51602,9 +51603,9 @@
       <c r="G849" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H849" s="2" t="e">
+      <c r="H849" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J849,SQL_LINEAGE!L849),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>330</v>
       </c>
       <c r="I849" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51659,9 +51660,9 @@
       <c r="G850" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H850" s="2" t="e">
+      <c r="H850" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J850,SQL_LINEAGE!L850),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>331</v>
       </c>
       <c r="I850" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51714,9 +51715,9 @@
       <c r="G851" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H851" s="2" t="e">
+      <c r="H851" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J851,SQL_LINEAGE!L851),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>331</v>
       </c>
       <c r="I851" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51769,9 +51770,9 @@
       <c r="G852" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="H852" s="2" t="e">
+      <c r="H852" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J852,SQL_LINEAGE!L852),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>331</v>
       </c>
       <c r="I852" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51826,9 +51827,9 @@
       <c r="G853" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H853" s="2" t="e">
+      <c r="H853" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J853,SQL_LINEAGE!L853),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>331</v>
       </c>
       <c r="I853" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51883,9 +51884,9 @@
       <c r="G854" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H854" s="2" t="e">
+      <c r="H854" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J854,SQL_LINEAGE!L854),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>332</v>
       </c>
       <c r="I854" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51938,9 +51939,9 @@
       <c r="G855" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H855" s="2" t="e">
+      <c r="H855" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J855,SQL_LINEAGE!L855),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>332</v>
       </c>
       <c r="I855" s="2" t="str">
         <f t="shared" si="34"/>
@@ -51993,9 +51994,9 @@
       <c r="G856" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H856" s="2" t="e">
+      <c r="H856" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J856,SQL_LINEAGE!L856),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>332</v>
       </c>
       <c r="I856" s="2" t="str">
         <f t="shared" si="34"/>
@@ -52050,9 +52051,9 @@
       <c r="G857" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H857" s="2" t="e">
+      <c r="H857" s="2">
         <f>VLOOKUP(_xlfn.CONCAT(J857,SQL_LINEAGE!L857),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>333</v>
       </c>
       <c r="I857" s="2" t="str">
         <f t="shared" si="34"/>
@@ -52106,8 +52107,9 @@
       <c r="G858" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="H858" s="13" t="e">
-        <v>#N/A</v>
+      <c r="H858" s="2">
+        <f>VLOOKUP(_xlfn.CONCAT(J858,SQL_LINEAGE!L858),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
+        <v>333</v>
       </c>
       <c r="I858" s="2" t="str">
         <f t="shared" si="34"/>
@@ -52161,8 +52163,9 @@
       <c r="G859" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="H859" s="13" t="e">
-        <v>#N/A</v>
+      <c r="H859" s="2">
+        <f>VLOOKUP(_xlfn.CONCAT(J859,SQL_LINEAGE!L859),SQL_LINEAGE_LABELS!$C$1:$D$994,2,FALSE)</f>
+        <v>333</v>
       </c>
       <c r="I859" s="2" t="str">
         <f t="shared" si="34"/>
@@ -52203,8 +52206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD88CCD7-C21C-486A-9478-C09BB5CBA6BC}">
   <dimension ref="A1:L594"/>
   <sheetViews>
-    <sheetView topLeftCell="A301" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B314" sqref="B314"/>
+    <sheetView topLeftCell="A323" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D324" sqref="D324:D335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57212,34 +57215,94 @@
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A330" s="1"/>
-      <c r="B330" s="5"/>
-      <c r="C330" s="2"/>
+      <c r="A330" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B330" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="C330" s="10" t="str">
+        <f>_xlfn.CONCAT(A330,B330)</f>
+        <v>ReportLatest_Time</v>
+      </c>
+      <c r="D330" s="5">
+        <v>328</v>
+      </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A331" s="1"/>
-      <c r="B331" s="5"/>
-      <c r="C331" s="2"/>
+      <c r="A331" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B331" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="C331" s="10" t="str">
+        <f t="shared" ref="C331:C335" si="6">_xlfn.CONCAT(A331,B331)</f>
+        <v>ReportCountry_Overview</v>
+      </c>
+      <c r="D331" s="5">
+        <v>329</v>
+      </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A332" s="1"/>
-      <c r="B332" s="5"/>
-      <c r="C332" s="2"/>
+      <c r="A332" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B332" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="C332" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>ReportTop5_Employees_Per_Product_Latest_Quarter</v>
+      </c>
+      <c r="D332" s="5">
+        <v>330</v>
+      </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A333" s="1"/>
-      <c r="B333" s="5"/>
-      <c r="C333" s="2"/>
+      <c r="A333" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B333" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C333" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>ReportTop5_Employees_Per_Order_Price_Latest_Month</v>
+      </c>
+      <c r="D333" s="5">
+        <v>331</v>
+      </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A334" s="1"/>
-      <c r="B334" s="5"/>
-      <c r="C334" s="2"/>
+      <c r="A334" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B334" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C334" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>ReportTop5_Employees_Per_Customer_Quantity_Latest_Year</v>
+      </c>
+      <c r="D334" s="5">
+        <v>332</v>
+      </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A335" s="1"/>
-      <c r="B335" s="5"/>
-      <c r="C335" s="2"/>
+      <c r="A335" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B335" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C335" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>ReportShipment_Overview</v>
+      </c>
+      <c r="D335" s="5">
+        <v>333</v>
+      </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A336" s="1"/>
@@ -58632,21 +58695,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C62DB221FDCFA7469315E52A99248468" ma:contentTypeVersion="7" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="a4b7b9417758175a3197062c1e9484c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="757fdb00-ad05-45d6-9096-306e7ca3eb9f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbe3202431c57f0f1e6b96cc39afc71d" ns3:_="">
     <xsd:import namespace="757fdb00-ad05-45d6-9096-306e7ca3eb9f"/>
@@ -58810,31 +58858,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD9A43C0-19CE-4F8E-8785-8744C71D4B93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="757fdb00-ad05-45d6-9096-306e7ca3eb9f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5542AFC4-889F-4E0B-9549-938C043F49F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B402AA0-FA6B-4C36-93BE-35C322F0EC0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -58850,4 +58889,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5542AFC4-889F-4E0B-9549-938C043F49F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD9A43C0-19CE-4F8E-8785-8744C71D4B93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="757fdb00-ad05-45d6-9096-306e7ca3eb9f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>